<commit_message>
"Performacer using REFramework - sprint 4"
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crossddelta\Documents\UiPath\process_emails_to_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2846B315-A49B-4909-AB39-663B51C94CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB54E538-3354-4E99-9230-EA607C8BAAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1488" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>"Mario Andre de Deus" &lt;profmario.deus@fiap.com.br&gt;</t>
-  </si>
-  <si>
     <t>Feedback Checkpoint #2 - 2o. semestre 2023</t>
   </si>
   <si>
@@ -47,15 +44,14 @@
     <t>CheckPoint 3 - Jogo-da-Velha Quântico</t>
   </si>
   <si>
-    <t xml:space="preserve">You have a Microsoft Teams assignment due by the end of this event._x000D_
-_x000D_
-View assignment &lt;https://teams.microsoft.com/l/entity/66aeee93-507d-479a-a3ef-8f494af43945/classroom?context=%7B%22subEntityId%22%3A%22%7B%5C%22version%5C%22%3A%5C%221.0%5C%22,%5C%22config%5C%22%3A%7B%5C%22classes%5C%22%3A%5B%7B%5C%22id%5C%22%3A%5C%225025c5c8-680c-44ad-acec-0606af9b2411%5C%22,%5C%22assignmentIds%5C%22%3A%5B%5C%226171af23-d4a0-4ef8-8967-7e1d44e5a082%5C%22%5D%7D%5D%7D,%5C%22action%5C%22%3A%5C%22navigate%5C%22,%5C%22view%5C%22%3A%5C%22assignment-viewer%5C%22,%5C%22deeplinkType%5C%22%3A2%7D%22,%22channelId%22%3Anull%7D&gt; _x000D_
-_x000D_
-Click for more information about this assignment._x000D_
-_x000D_
-_x000D_
-Learn more &lt;https://support.microsoft.com/topic/7cb294be-2c63-4f2d-acf2-299329bcd5bf&gt;  | All assignments &lt;https://teams.microsoft.com/l/entity/66aeee93-507d-479a-a3ef-8f494af43945/classroom?context=%7b%22channelId%22%3anull%7d&gt; _x000D_
+    <t xml:space="preserve">You have a Microsoft Teams assignment due by the end of this event.
+View assignment &lt;https://teams.microsoft.com/l/entity/66aeee93-507d-479a-a3ef-8f494af43945/classroom?context=%7B%22subEntityId%22%3A%22%7B%5C%22version%5C%22%3A%5C%221.0%5C%22,%5C%22config%5C%22%3A%7B%5C%22classes%5C%22%3A%5B%7B%5C%22id%5C%22%3A%5C%225025c5c8-680c-44ad-acec-0606af9b2411%5C%22,%5C%22assignmentIds%5C%22%3A%5B%5C%226171af23-d4a0-4ef8-8967-7e1d44e5a082%5C%22%5D%7D%5D%7D,%5C%22action%5C%22%3A%5C%22navigate%5C%22,%5C%22view%5C%22%3A%5C%22assignment-viewer%5C%22,%5C%22deeplinkType%5C%22%3A2%7D%22,%22channelId%22%3Anull%7D&gt; 
+Click for more information about this assignment.
+Learn more &lt;https://support.microsoft.com/topic/7cb294be-2c63-4f2d-acf2-299329bcd5bf&gt;  | All assignments &lt;https://teams.microsoft.com/l/entity/66aeee93-507d-479a-a3ef-8f494af43945/classroom?context=%7b%22channelId%22%3anull%7d&gt; 
 </t>
+  </si>
+  <si>
+    <t>"professor autoML" &lt;prof.deus@fiap.com.br&gt;</t>
   </si>
 </sst>
 </file>
@@ -378,35 +374,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>